<commit_message>
+ multifile for handlers
</commit_message>
<xml_diff>
--- a/excel_parser/questions.xlsx
+++ b/excel_parser/questions.xlsx
@@ -4,17 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$1:$C$33</definedName>
+  </definedNames>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="63">
   <si>
     <t>Вопрос, который бот задаст представителю компании</t>
   </si>
@@ -38,7 +41,172 @@
 Продукт (фокусный продукт, на развитие которого привлекаются инвестиции) (1-2 предложения)</t>
   </si>
   <si>
+    <t>image</t>
+  </si>
+  <si>
     <t>feature</t>
+  </si>
+  <si>
+    <t>Введите название вашего стартапа</t>
+  </si>
+  <si>
+    <t>name_project</t>
+  </si>
+  <si>
+    <t>about_project</t>
+  </si>
+  <si>
+    <t>Краткое описание Вашего стартапа (2 - 3 предложения)</t>
+  </si>
+  <si>
+    <t>еffectiveness</t>
+  </si>
+  <si>
+    <t>Опишите основной эффект от использования Вашей идеи</t>
+  </si>
+  <si>
+    <t>Выделите 2-3 основные цели Вашего стартапа</t>
+  </si>
+  <si>
+    <t>goals</t>
+  </si>
+  <si>
+    <t>risks</t>
+  </si>
+  <si>
+    <t>Возможные негативные эффекты от Вашего стартапа</t>
+  </si>
+  <si>
+    <t>teammate1</t>
+  </si>
+  <si>
+    <t>teammate2</t>
+  </si>
+  <si>
+    <t>teammate3</t>
+  </si>
+  <si>
+    <t>teammate4</t>
+  </si>
+  <si>
+    <t>Сколько примерно человек в штате? (в следующих вопросах Вам будет необходимо их представить)</t>
+  </si>
+  <si>
+    <t>team</t>
+  </si>
+  <si>
+    <t>Фамилия И.О., Должность, Опыт</t>
+  </si>
+  <si>
+    <t>Фамилия И.О., Должность, Опыт  (чтобы пропустить вопрос напишите "-")</t>
+  </si>
+  <si>
+    <t>first_stage</t>
+  </si>
+  <si>
+    <t>Опишите (пару слов) о данном этапе</t>
+  </si>
+  <si>
+    <t>Опишите конечный результат Вашего стартапа</t>
+  </si>
+  <si>
+    <t>problems</t>
+  </si>
+  <si>
+    <t>Напишите актуальность Вашего сартапа</t>
+  </si>
+  <si>
+    <t>Инструменты для реализации Вашего решения (пару слов)</t>
+  </si>
+  <si>
+    <t>strategy</t>
+  </si>
+  <si>
+    <t>decision</t>
+  </si>
+  <si>
+    <t>final_stage_discription</t>
+  </si>
+  <si>
+    <t>final_stage</t>
+  </si>
+  <si>
+    <t>third_stage_discription</t>
+  </si>
+  <si>
+    <t>third_stage</t>
+  </si>
+  <si>
+    <t>second_stage_discription</t>
+  </si>
+  <si>
+    <t>second_stage</t>
+  </si>
+  <si>
+    <t>first_stage_description</t>
+  </si>
+  <si>
+    <t>Что даёт возможность реализовать Ваш стартап?</t>
+  </si>
+  <si>
+    <t>forecast</t>
+  </si>
+  <si>
+    <t>Каков прогноз Вашего стартапа? (фотография где сравниваются Ваша стратегия с текущим положением рынка)</t>
+  </si>
+  <si>
+    <t>Фотография сотрудника</t>
+  </si>
+  <si>
+    <t>teammate1_photo</t>
+  </si>
+  <si>
+    <t>teammate2_photo</t>
+  </si>
+  <si>
+    <t>teammate3_photo</t>
+  </si>
+  <si>
+    <t>teammate4_photo</t>
+  </si>
+  <si>
+    <t>picture1</t>
+  </si>
+  <si>
+    <t>picture2</t>
+  </si>
+  <si>
+    <t>Напишите описание к первой фотографии</t>
+  </si>
+  <si>
+    <t>Напишите описание к второй фотографии</t>
+  </si>
+  <si>
+    <t>descript_picture1</t>
+  </si>
+  <si>
+    <t>descript_picture2</t>
+  </si>
+  <si>
+    <t>Загрузите первую фотографию Вашего решения (Всего фотографий 2)</t>
+  </si>
+  <si>
+    <t>Загрузите вторую фотографию Вашего решения</t>
+  </si>
+  <si>
+    <t>Напишите примерную дату первого этапа Вашего стартапа (Всего этапов будет 4)</t>
+  </si>
+  <si>
+    <t>Напишите примерную дату второго этапа Вашего стартапа</t>
+  </si>
+  <si>
+    <t>Напишите примерную дату третьего этапа Вашего стартапа</t>
+  </si>
+  <si>
+    <t>Напишите примерную дату заключающего этапа Вашего стартапа</t>
+  </si>
+  <si>
+    <t>Фотография сотрудника (чтобы пропустить вопрос напишите "-")</t>
   </si>
 </sst>
 </file>
@@ -541,20 +709,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="100.7109375" style="10" customWidth="1"/>
-    <col min="2" max="2" width="42.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="100.6640625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="42.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -565,29 +733,360 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="C3" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="4" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C33"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
+ pdf and excel sheets
</commit_message>
<xml_diff>
--- a/excel_parser/questions.xlsx
+++ b/excel_parser/questions.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13890" windowHeight="4560"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13890" windowHeight="4560" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист2" sheetId="2" r:id="rId2"/>
+    <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="107">
   <si>
     <t>Вопрос, который бот задаст представителю компании</t>
   </si>
@@ -782,8 +784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1010"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1105,7 +1107,7 @@
       </c>
       <c r="D26" s="6"/>
     </row>
-    <row r="27" spans="1:4" ht="29.25" customHeight="1">
+    <row r="27" spans="1:4">
       <c r="A27" s="7" t="s">
         <v>50</v>
       </c>
@@ -1117,7 +1119,7 @@
       </c>
       <c r="D27" s="6"/>
     </row>
-    <row r="28" spans="1:4" ht="29.25" customHeight="1">
+    <row r="28" spans="1:4">
       <c r="A28" s="7" t="s">
         <v>48</v>
       </c>
@@ -6065,4 +6067,143 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="72.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="30">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="30">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>